<commit_message>
Corrección bug carga masiva
</commit_message>
<xml_diff>
--- a/SW.CEMENTERIO/SW.CEMENTERIO/wwwroot/assets/Plantillas/PLANTILLA_PABELLON_NICHOS.xlsx
+++ b/SW.CEMENTERIO/SW.CEMENTERIO/wwwroot/assets/Plantillas/PLANTILLA_PABELLON_NICHOS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Archivos\UTP\VIII CICLO\INTEGRADOR I\GIT\Cementerio\SW.CEMENTERIO\SW.CEMENTERIO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Archivos\UTP\VIII CICLO\INTEGRADOR I\GIT\Cementerio\SW.CEMENTERIO\SW.CEMENTERIO\wwwroot\assets\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{233E95A1-FC76-4EA1-B18D-6D13687573B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901ADCCC-0DDD-4536-9B25-6BA73C78EE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CD951F68-319D-4B25-B2BC-4C5CC27A5460}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,21 +82,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -124,7 +110,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,20 +440,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE04E8C-E0B2-42C5-BD71-90317AC72FBD}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D21"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,128 +468,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>